<commit_message>
Updated Studies, including Stocks Quotes
</commit_message>
<xml_diff>
--- a/rows/req.xlsx
+++ b/rows/req.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maion/OneDrive/Documentos/Documentos Felipe/programs/ruby/Python/PyCharmProjects/testes/rows/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81f1bd838ef35b84/Documentos/Documentos Felipe/programs/ruby/Python/PyCharmProjects/testes/rows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{733567E0-E700-A64B-9683-7A4A92F2B3B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B99CA480-A1BF-8E4F-96E1-B9DEA999635B}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{733567E0-E700-A64B-9683-7A4A92F2B3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B08E0D1B-F88C-BC44-B36B-98D733C85202}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="24940" windowHeight="14980" activeTab="2" xr2:uid="{15604F96-AAC6-C043-A8E8-3C18D3E0E199}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Processo</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>LISTA DE LICENÇAS AMBIENTAIS REQUERIDAS</t>
+  </si>
+  <si>
+    <t>kld;jicvxsp'[\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">][][[VB==0PB[-OP NKS   </t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>V ,;/.C</t>
   </si>
 </sst>
 </file>
@@ -169,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,6 +211,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +598,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5255D9C-C957-9548-B35E-0D81408A99CF}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="101" workbookViewId="0">
+      <selection activeCell="C3" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,7 +609,7 @@
     <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -604,7 +617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -612,25 +625,46 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>